<commit_message>
Latest changes but gave up because of missing functionality.
</commit_message>
<xml_diff>
--- a/_templates/Digital-Bulletin-Board/Social_Media_KPI.xlsx
+++ b/_templates/Digital-Bulletin-Board/Social_Media_KPI.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Digital-Bulletin-Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C96EA4B8-9220-C948-AF51-FD861C7893C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D3F4E0-84FD-E944-8AED-131D565B1AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-56820" yWindow="80" windowWidth="26220" windowHeight="16140" xr2:uid="{FA8DD709-2215-8F4D-BC37-EB83C48D08E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Channel</t>
   </si>
@@ -53,16 +53,13 @@
     <t>Facebook</t>
   </si>
   <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
     <t>Follower</t>
-  </si>
-  <si>
-    <t>Likes</t>
-  </si>
-  <si>
-    <t>Twitter</t>
-  </si>
-  <si>
-    <t>Instagram</t>
   </si>
 </sst>
 </file>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0AF83D-6E7E-FF45-9B36-A7E8924113DA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>24561</v>
@@ -459,55 +456,37 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>246</v>
+        <v>4654</v>
       </c>
       <c r="D3">
-        <v>843</v>
+        <v>4684</v>
       </c>
       <c r="E3">
         <f>C3-D3</f>
-        <v>-597</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
       <c r="C4">
-        <v>4654</v>
+        <v>5416</v>
       </c>
       <c r="D4">
-        <v>4564</v>
+        <v>4683</v>
       </c>
       <c r="E4">
         <f>C4-D4</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>5416</v>
-      </c>
-      <c r="D5">
-        <v>4683</v>
-      </c>
-      <c r="E5">
-        <f>C5-D5</f>
         <v>733</v>
       </c>
     </row>

</xml_diff>